<commit_message>
Make the distinction between runtime and localisation/recording files.
</commit_message>
<xml_diff>
--- a/examples/main-strings.xlsx
+++ b/examples/main-strings.xlsx
@@ -40,6 +40,24 @@
     <x:t/>
   </x:si>
   <x:si>
+    <x:t>scene1_Scene1_Part1_621G</x:t>
+  </x:si>
+  <x:si>
+    <x:t>With several lines.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>scene1_Scene1_Part2_N5RW</x:t>
+  </x:si>
+  <x:si>
+    <x:t>And here's part 2.</x:t>
+  </x:si>
+  <x:si>
+    <x:t>scene1_Scene1_Part3_UZOH</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Dave walks into the room.</x:t>
+  </x:si>
+  <x:si>
     <x:t>scene1_Scene1_Part3_9MXL</x:t>
   </x:si>
   <x:si>
@@ -94,12 +112,24 @@
     <x:t>GEORGE</x:t>
   </x:si>
   <x:si>
+    <x:t>scene1_Scene1_Right_3V6T</x:t>
+  </x:si>
+  <x:si>
+    <x:t>George swerves the car right.</x:t>
+  </x:si>
+  <x:si>
     <x:t>scene1_Scene1_Right_WM69</x:t>
   </x:si>
   <x:si>
     <x:t>You sure you want to go right?</x:t>
   </x:si>
   <x:si>
+    <x:t>scene1_Scene1_Left_HZ7B</x:t>
+  </x:si>
+  <x:si>
+    <x:t>George swerves the car left.</x:t>
+  </x:si>
+  <x:si>
     <x:t>scene1_Scene1_Left_MIM6</x:t>
   </x:si>
   <x:si>
@@ -142,6 +172,18 @@
     <x:t>This is a loud line!</x:t>
   </x:si>
   <x:si>
+    <x:t>main_TestScene_79PN</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Now bounce around the place!</x:t>
+  </x:si>
+  <x:si>
+    <x:t>main_TestScene_96IR</x:t>
+  </x:si>
+  <x:si>
+    <x:t>(SFX) Make a bang noise!</x:t>
+  </x:si>
+  <x:si>
     <x:t>main_TestScene_IQIS</x:t>
   </x:si>
   <x:si>
@@ -164,6 +206,12 @@
   </x:si>
   <x:si>
     <x:t>Bark3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>main_Barks_046M</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Testing a normal line.</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_JFG1</x:t>
@@ -274,8 +322,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D25" totalsRowShown="0">
-  <x:autoFilter ref="A1:D25"/>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D33" totalsRowShown="0">
+  <x:autoFilter ref="A1:D33"/>
   <x:tableColumns count="4">
     <x:tableColumn id="1" name="ID"/>
     <x:tableColumn id="2" name="Text"/>
@@ -574,7 +622,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:D25"/>
+  <x:dimension ref="A1:D33"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -622,7 +670,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="C3" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D3" s="0" t="s">
         <x:v>7</x:v>
@@ -630,10 +678,10 @@
     </x:row>
     <x:row r="4" spans="1:4">
       <x:c r="A4" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
         <x:v>11</x:v>
-      </x:c>
-      <x:c r="B4" s="0" t="s">
-        <x:v>12</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
         <x:v>7</x:v>
@@ -644,13 +692,13 @@
     </x:row>
     <x:row r="5" spans="1:4">
       <x:c r="A5" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="B5" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D5" s="0" t="s">
         <x:v>7</x:v>
@@ -658,13 +706,13 @@
     </x:row>
     <x:row r="6" spans="1:4">
       <x:c r="A6" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="B6" s="0" t="s">
+      <x:c r="C6" s="0" t="s">
         <x:v>16</x:v>
-      </x:c>
-      <x:c r="C6" s="0" t="s">
-        <x:v>7</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
         <x:v>7</x:v>
@@ -678,7 +726,7 @@
         <x:v>18</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
         <x:v>7</x:v>
@@ -692,7 +740,7 @@
         <x:v>20</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
         <x:v>7</x:v>
@@ -706,7 +754,7 @@
         <x:v>22</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
         <x:v>7</x:v>
@@ -720,7 +768,7 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
         <x:v>7</x:v>
@@ -728,13 +776,13 @@
     </x:row>
     <x:row r="11" spans="1:4">
       <x:c r="A11" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="B11" s="0" t="s">
-        <x:v>27</x:v>
-      </x:c>
       <x:c r="C11" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
         <x:v>7</x:v>
@@ -742,13 +790,13 @@
     </x:row>
     <x:row r="12" spans="1:4">
       <x:c r="A12" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="B12" s="0" t="s">
         <x:v>28</x:v>
       </x:c>
-      <x:c r="B12" s="0" t="s">
-        <x:v>29</x:v>
-      </x:c>
       <x:c r="C12" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
         <x:v>7</x:v>
@@ -756,13 +804,13 @@
     </x:row>
     <x:row r="13" spans="1:4">
       <x:c r="A13" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="B13" s="0" t="s">
         <x:v>30</x:v>
       </x:c>
-      <x:c r="B13" s="0" t="s">
+      <x:c r="C13" s="0" t="s">
         <x:v>31</x:v>
-      </x:c>
-      <x:c r="C13" s="0" t="s">
-        <x:v>7</x:v>
       </x:c>
       <x:c r="D13" s="0" t="s">
         <x:v>7</x:v>
@@ -790,7 +838,7 @@
         <x:v>35</x:v>
       </x:c>
       <x:c r="C15" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="D15" s="0" t="s">
         <x:v>7</x:v>
@@ -798,27 +846,27 @@
     </x:row>
     <x:row r="16" spans="1:4">
       <x:c r="A16" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="B16" s="0" t="s">
         <x:v>37</x:v>
       </x:c>
-      <x:c r="B16" s="0" t="s">
-        <x:v>38</x:v>
-      </x:c>
       <x:c r="C16" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D16" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>7</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:4">
       <x:c r="A17" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="C17" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="D17" s="0" t="s">
         <x:v>7</x:v>
@@ -826,13 +874,13 @@
     </x:row>
     <x:row r="18" spans="1:4">
       <x:c r="A18" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="C18" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D18" s="0" t="s">
         <x:v>7</x:v>
@@ -840,13 +888,13 @@
     </x:row>
     <x:row r="19" spans="1:4">
       <x:c r="A19" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="B19" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="C19" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D19" s="0" t="s">
         <x:v>7</x:v>
@@ -854,13 +902,13 @@
     </x:row>
     <x:row r="20" spans="1:4">
       <x:c r="A20" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="B20" s="0" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="C20" s="0" t="s">
         <x:v>46</x:v>
-      </x:c>
-      <x:c r="B20" s="0" t="s">
-        <x:v>47</x:v>
-      </x:c>
-      <x:c r="C20" s="0" t="s">
-        <x:v>6</x:v>
       </x:c>
       <x:c r="D20" s="0" t="s">
         <x:v>7</x:v>
@@ -868,16 +916,16 @@
     </x:row>
     <x:row r="21" spans="1:4">
       <x:c r="A21" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="B21" s="0" t="s">
         <x:v>48</x:v>
       </x:c>
-      <x:c r="B21" s="0" t="s">
+      <x:c r="C21" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="D21" s="0" t="s">
         <x:v>49</x:v>
-      </x:c>
-      <x:c r="C21" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="D21" s="0" t="s">
-        <x:v>7</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:4">
@@ -902,7 +950,7 @@
         <x:v>53</x:v>
       </x:c>
       <x:c r="C23" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D23" s="0" t="s">
         <x:v>7</x:v>
@@ -910,13 +958,13 @@
     </x:row>
     <x:row r="24" spans="1:4">
       <x:c r="A24" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="B24" s="0" t="s">
         <x:v>55</x:v>
       </x:c>
-      <x:c r="B24" s="0" t="s">
-        <x:v>56</x:v>
-      </x:c>
       <x:c r="C24" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D24" s="0" t="s">
         <x:v>7</x:v>
@@ -924,15 +972,127 @@
     </x:row>
     <x:row r="25" spans="1:4">
       <x:c r="A25" s="0" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="B25" s="0" t="s">
         <x:v>57</x:v>
-      </x:c>
-      <x:c r="B25" s="0" t="s">
-        <x:v>58</x:v>
       </x:c>
       <x:c r="C25" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
       <x:c r="D25" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26" spans="1:4">
+      <x:c r="A26" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="B26" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="C26" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D26" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="1:4">
+      <x:c r="A27" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="B27" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="C27" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D27" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28" spans="1:4">
+      <x:c r="A28" s="0" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="B28" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="C28" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D28" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="1:4">
+      <x:c r="A29" s="0" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="B29" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="C29" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D29" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="30" spans="1:4">
+      <x:c r="A30" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="B30" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="C30" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D30" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="31" spans="1:4">
+      <x:c r="A31" s="0" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="B31" s="0" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="C31" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="D31" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="32" spans="1:4">
+      <x:c r="A32" s="0" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="B32" s="0" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="C32" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D32" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="33" spans="1:4">
+      <x:c r="A33" s="0" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="B33" s="0" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="C33" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="D33" s="0" t="s">
         <x:v>7</x:v>
       </x:c>
     </x:row>

</xml_diff>

<commit_message>
Add project file concept, rejig configuration.
</commit_message>
<xml_diff>
--- a/examples/main-strings.xlsx
+++ b/examples/main-strings.xlsx
@@ -6,7 +6,7 @@
     <x:workbookView firstSheet="0" activeTab="0"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Voice Lines - main" sheetId="1" r:id="rId2"/>
+    <x:sheet name="Text Lines - main" sheetId="1" r:id="rId2"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="125725"/>
@@ -40,24 +40,6 @@
     <x:t/>
   </x:si>
   <x:si>
-    <x:t>scene1_Scene1_Part1_621G</x:t>
-  </x:si>
-  <x:si>
-    <x:t>With several lines.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>scene1_Scene1_Part2_N5RW</x:t>
-  </x:si>
-  <x:si>
-    <x:t>And here's part 2.</x:t>
-  </x:si>
-  <x:si>
-    <x:t>scene1_Scene1_Part3_UZOH</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Dave walks into the room.</x:t>
-  </x:si>
-  <x:si>
     <x:t>scene1_Scene1_Part3_9MXL</x:t>
   </x:si>
   <x:si>
@@ -112,24 +94,12 @@
     <x:t>GEORGE</x:t>
   </x:si>
   <x:si>
-    <x:t>scene1_Scene1_Right_3V6T</x:t>
-  </x:si>
-  <x:si>
-    <x:t>George swerves the car right.</x:t>
-  </x:si>
-  <x:si>
     <x:t>scene1_Scene1_Right_WM69</x:t>
   </x:si>
   <x:si>
     <x:t>You sure you want to go right?</x:t>
   </x:si>
   <x:si>
-    <x:t>scene1_Scene1_Left_HZ7B</x:t>
-  </x:si>
-  <x:si>
-    <x:t>George swerves the car left.</x:t>
-  </x:si>
-  <x:si>
     <x:t>scene1_Scene1_Left_MIM6</x:t>
   </x:si>
   <x:si>
@@ -172,18 +142,6 @@
     <x:t>This is a loud line!</x:t>
   </x:si>
   <x:si>
-    <x:t>main_TestScene_79PN</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Now bounce around the place!</x:t>
-  </x:si>
-  <x:si>
-    <x:t>main_TestScene_96IR</x:t>
-  </x:si>
-  <x:si>
-    <x:t>(SFX) Make a bang noise!</x:t>
-  </x:si>
-  <x:si>
     <x:t>main_TestScene_IQIS</x:t>
   </x:si>
   <x:si>
@@ -206,12 +164,6 @@
   </x:si>
   <x:si>
     <x:t>Bark3</x:t>
-  </x:si>
-  <x:si>
-    <x:t>main_Barks_046M</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Testing a normal line.</x:t>
   </x:si>
   <x:si>
     <x:t>main_Barks_JFG1</x:t>
@@ -322,8 +274,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D33" totalsRowShown="0">
-  <x:autoFilter ref="A1:D33"/>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D25" totalsRowShown="0">
+  <x:autoFilter ref="A1:D25"/>
   <x:tableColumns count="4">
     <x:tableColumn id="1" name="ID"/>
     <x:tableColumn id="2" name="Text"/>
@@ -622,7 +574,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:D33"/>
+  <x:dimension ref="A1:D25"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -670,7 +622,7 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="C3" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="D3" s="0" t="s">
         <x:v>7</x:v>
@@ -678,10 +630,10 @@
     </x:row>
     <x:row r="4" spans="1:4">
       <x:c r="A4" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
         <x:v>7</x:v>
@@ -692,13 +644,13 @@
     </x:row>
     <x:row r="5" spans="1:4">
       <x:c r="A5" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D5" s="0" t="s">
         <x:v>7</x:v>
@@ -706,13 +658,13 @@
     </x:row>
     <x:row r="6" spans="1:4">
       <x:c r="A6" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
         <x:v>7</x:v>
@@ -726,7 +678,7 @@
         <x:v>18</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
         <x:v>7</x:v>
@@ -740,7 +692,7 @@
         <x:v>20</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
         <x:v>7</x:v>
@@ -754,7 +706,7 @@
         <x:v>22</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
         <x:v>7</x:v>
@@ -768,7 +720,7 @@
         <x:v>24</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
         <x:v>7</x:v>
@@ -776,13 +728,13 @@
     </x:row>
     <x:row r="11" spans="1:4">
       <x:c r="A11" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="C11" s="0" t="s">
         <x:v>25</x:v>
-      </x:c>
-      <x:c r="B11" s="0" t="s">
-        <x:v>26</x:v>
-      </x:c>
-      <x:c r="C11" s="0" t="s">
-        <x:v>7</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
         <x:v>7</x:v>
@@ -790,13 +742,13 @@
     </x:row>
     <x:row r="12" spans="1:4">
       <x:c r="A12" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
         <x:v>7</x:v>
@@ -804,13 +756,13 @@
     </x:row>
     <x:row r="13" spans="1:4">
       <x:c r="A13" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="C13" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="D13" s="0" t="s">
         <x:v>7</x:v>
@@ -838,7 +790,7 @@
         <x:v>35</x:v>
       </x:c>
       <x:c r="C15" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="D15" s="0" t="s">
         <x:v>7</x:v>
@@ -846,27 +798,27 @@
     </x:row>
     <x:row r="16" spans="1:4">
       <x:c r="A16" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="B16" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="C16" s="0" t="s">
         <x:v>36</x:v>
       </x:c>
-      <x:c r="B16" s="0" t="s">
-        <x:v>37</x:v>
-      </x:c>
-      <x:c r="C16" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
       <x:c r="D16" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>39</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:4">
       <x:c r="A17" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="C17" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D17" s="0" t="s">
         <x:v>7</x:v>
@@ -874,13 +826,13 @@
     </x:row>
     <x:row r="18" spans="1:4">
       <x:c r="A18" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="C18" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D18" s="0" t="s">
         <x:v>7</x:v>
@@ -888,13 +840,13 @@
     </x:row>
     <x:row r="19" spans="1:4">
       <x:c r="A19" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="B19" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="C19" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D19" s="0" t="s">
         <x:v>7</x:v>
@@ -902,13 +854,13 @@
     </x:row>
     <x:row r="20" spans="1:4">
       <x:c r="A20" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="B20" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="C20" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D20" s="0" t="s">
         <x:v>7</x:v>
@@ -916,16 +868,16 @@
     </x:row>
     <x:row r="21" spans="1:4">
       <x:c r="A21" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="C21" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D21" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>7</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:4">
@@ -950,7 +902,7 @@
         <x:v>53</x:v>
       </x:c>
       <x:c r="C23" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="D23" s="0" t="s">
         <x:v>7</x:v>
@@ -958,13 +910,13 @@
     </x:row>
     <x:row r="24" spans="1:4">
       <x:c r="A24" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="B24" s="0" t="s">
-        <x:v>55</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="C24" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="D24" s="0" t="s">
         <x:v>7</x:v>
@@ -972,127 +924,15 @@
     </x:row>
     <x:row r="25" spans="1:4">
       <x:c r="A25" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="B25" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="C25" s="0" t="s">
         <x:v>6</x:v>
       </x:c>
       <x:c r="D25" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="26" spans="1:4">
-      <x:c r="A26" s="0" t="s">
-        <x:v>58</x:v>
-      </x:c>
-      <x:c r="B26" s="0" t="s">
-        <x:v>59</x:v>
-      </x:c>
-      <x:c r="C26" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="D26" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="27" spans="1:4">
-      <x:c r="A27" s="0" t="s">
-        <x:v>60</x:v>
-      </x:c>
-      <x:c r="B27" s="0" t="s">
-        <x:v>61</x:v>
-      </x:c>
-      <x:c r="C27" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="D27" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="28" spans="1:4">
-      <x:c r="A28" s="0" t="s">
-        <x:v>62</x:v>
-      </x:c>
-      <x:c r="B28" s="0" t="s">
-        <x:v>63</x:v>
-      </x:c>
-      <x:c r="C28" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="D28" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="29" spans="1:4">
-      <x:c r="A29" s="0" t="s">
-        <x:v>64</x:v>
-      </x:c>
-      <x:c r="B29" s="0" t="s">
-        <x:v>65</x:v>
-      </x:c>
-      <x:c r="C29" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D29" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="30" spans="1:4">
-      <x:c r="A30" s="0" t="s">
-        <x:v>66</x:v>
-      </x:c>
-      <x:c r="B30" s="0" t="s">
-        <x:v>67</x:v>
-      </x:c>
-      <x:c r="C30" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="D30" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="31" spans="1:4">
-      <x:c r="A31" s="0" t="s">
-        <x:v>68</x:v>
-      </x:c>
-      <x:c r="B31" s="0" t="s">
-        <x:v>69</x:v>
-      </x:c>
-      <x:c r="C31" s="0" t="s">
-        <x:v>70</x:v>
-      </x:c>
-      <x:c r="D31" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="32" spans="1:4">
-      <x:c r="A32" s="0" t="s">
-        <x:v>71</x:v>
-      </x:c>
-      <x:c r="B32" s="0" t="s">
-        <x:v>72</x:v>
-      </x:c>
-      <x:c r="C32" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="D32" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="33" spans="1:4">
-      <x:c r="A33" s="0" t="s">
-        <x:v>73</x:v>
-      </x:c>
-      <x:c r="B33" s="0" t="s">
-        <x:v>74</x:v>
-      </x:c>
-      <x:c r="C33" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="D33" s="0" t="s">
         <x:v>7</x:v>
       </x:c>
     </x:row>

</xml_diff>